<commit_message>
ST-0013: added in answer for question 1, 2, 3, and 5
</commit_message>
<xml_diff>
--- a/InmateRosterDataFolder/Inmate Program Data.xlsx
+++ b/InmateRosterDataFolder/Inmate Program Data.xlsx
@@ -3,8 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="INMATEROSTERDATA" sheetId="1" r:id="rId5"/>
-    <sheet state="visible" name="PROGRAMDATA" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="MASTER" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="IPPEXPN" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Question 1" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Question 2" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Question 3" sheetId="5" r:id="rId9"/>
+    <sheet state="visible" name="Question 5" sheetId="6" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>MASDC#</t>
   </si>
@@ -35,18 +39,21 @@
     <t>John Smith</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Facility A</t>
+  </si>
+  <si>
+    <t>Unit 1</t>
+  </si>
+  <si>
+    <t>Robert Lee</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
-    <t>Facility A</t>
-  </si>
-  <si>
-    <t>Unit 1</t>
-  </si>
-  <si>
-    <t>Robert Lee</t>
-  </si>
-  <si>
     <t>Facility B</t>
   </si>
   <si>
@@ -56,15 +63,15 @@
     <t xml:space="preserve">Michael Brown </t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>Unit 2</t>
   </si>
   <si>
     <t>David Johnson</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Facility C</t>
   </si>
   <si>
@@ -83,28 +90,31 @@
     <t>Daniel Anderson</t>
   </si>
   <si>
+    <t>Facility D</t>
+  </si>
+  <si>
+    <t>Alex Han</t>
+  </si>
+  <si>
     <t>EXPNDCN</t>
   </si>
   <si>
     <t>EXPNDSC</t>
   </si>
   <si>
+    <t>EXPNNCR</t>
+  </si>
+  <si>
     <t>EXPPSTAT</t>
   </si>
   <si>
-    <t>EXPNNCR</t>
-  </si>
-  <si>
     <t>Sex Offender</t>
   </si>
   <si>
     <t>I</t>
   </si>
   <si>
-    <t>Traffic Violdation</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>Traffic Violation</t>
   </si>
   <si>
     <t>Shoplifting</t>
@@ -144,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -160,6 +170,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -220,13 +231,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle count="4" pivot="0" name="INMATEROSTERDATA-style">
+    <tableStyle count="4" pivot="0" name="MASTER-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
-    <tableStyle count="4" pivot="0" name="PROGRAMDATA-style">
+    <tableStyle count="4" pivot="0" name="IPPEXPN-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -244,12 +255,28 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F8" displayName="Sample_Inmate_Roster_Data" name="Sample_Inmate_Roster_Data" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F9" displayName="MASTER" name="MASTER" id="1">
   <tableColumns count="6">
     <tableColumn name="MASDC#" id="1"/>
     <tableColumn name="MASCNM" id="2"/>
@@ -258,19 +285,19 @@
     <tableColumn name="MASLC3" id="5"/>
     <tableColumn name="MASSOFF" id="6"/>
   </tableColumns>
-  <tableStyleInfo name="INMATEROSTERDATA-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="MASTER-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D9" displayName="Sample_Program_Data" name="Sample_Program_Data" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D9" displayName="IPPEXPN" name="IPPEXPN" id="2">
   <tableColumns count="4">
     <tableColumn name="EXPNDCN" id="1"/>
     <tableColumn name="EXPNDSC" id="2"/>
-    <tableColumn name="EXPPSTAT" id="3"/>
-    <tableColumn name="EXPNNCR" id="4"/>
+    <tableColumn name="EXPNNCR" id="3"/>
+    <tableColumn name="EXPPSTAT" id="4"/>
   </tableColumns>
-  <tableStyleInfo name="PROGRAMDATA-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="IPPEXPN-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -523,6 +550,7 @@
       <c r="F2" s="3">
         <v>1.0</v>
       </c>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3">
@@ -532,13 +560,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3">
         <v>1.0</v>
@@ -549,16 +577,16 @@
         <v>1003.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3">
         <v>0.0</v>
@@ -569,19 +597,19 @@
         <v>1004.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
@@ -589,16 +617,16 @@
         <v>1005.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3">
         <v>1.0</v>
@@ -609,16 +637,16 @@
         <v>1006.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3">
         <v>1.0</v>
@@ -629,25 +657,40 @@
         <v>1007.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3">
         <v>1.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="3">
+        <v>1008.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -671,22 +714,22 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="18.38"/>
-    <col customWidth="1" min="3" max="3" width="10.38"/>
-    <col customWidth="1" min="4" max="4" width="11.88"/>
+    <col customWidth="1" min="3" max="3" width="15.13"/>
+    <col customWidth="1" min="4" max="4" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
@@ -694,41 +737,41 @@
         <v>1001.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
+        <v>30</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="3">
-        <v>1001.0</v>
+        <v>1002.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
+        <v>32</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="3">
-        <v>1002.0</v>
+        <v>1003.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.0</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
@@ -736,13 +779,13 @@
         <v>1004.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
@@ -750,13 +793,13 @@
         <v>1005.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.0</v>
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
@@ -764,13 +807,13 @@
         <v>1006.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3">
         <v>1.0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" ht="22.5" customHeight="1">
@@ -778,27 +821,27 @@
         <v>1007.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3">
-        <v>1.0</v>
+      <c r="C8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="3">
-        <v>1007.0</v>
+        <v>1008.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -807,4 +850,266 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(
+  MASTER!B2:B1005,
+  MASTER!F2:F1005 = 1,
+  MASTER!C2:C1005 = ""A"",
+    MATCH(
+      MASTER!A2:A1005,
+      FILTER(
+        IPPEXPN!A2:A1005,
+        IPPEXPN!C2:C1005 = 1,
+        REGEXMATCH(IPPEXPN!B2:B1005, ""Sex Offender"")
+      )
+  )
+)
+"),"Robert Lee")</f>
+        <v>Robert Lee</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Daniel Anderson")</f>
+        <v>Daniel Anderson</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Alex Han")</f>
+        <v>Alex Han</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
+  FILTER(
+    {
+      MASTER!D2:D1000,
+      MASTER!A2:A1000
+    },
+    MASTER!F2:F1000 = 1,
+    MASTER!C2:C1000 = ""A"",
+    MATCH(
+      MASTER!A2:A1000,
+      FILTER(
+        IPPEXPN!A2:A1000,
+        IPPEXPN!C2:C1000 = 1,
+        IPPEXPN!D2:D10"&amp;"00 &lt;&gt; 1,
+        REGEXMATCH(IPPEXPN!B2:B1000, ""Sex Offender"")
+      )
+    )
+  ),
+  ""SELECT Col1, COUNT(Col2)
+   GROUP BY Col1
+   LABEL Col1 'Facility',
+         COUNT(Col2) 'Offenders Without Credit'""
+)"),"Facility")</f>
+        <v>Facility</v>
+      </c>
+      <c r="B1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Offenders Without Credit")</f>
+        <v>Offenders Without Credit</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
+        <v>Facility A</v>
+      </c>
+      <c r="B2" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility B")</f>
+        <v>Facility B</v>
+      </c>
+      <c r="B3" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility D")</f>
+        <v>Facility D</v>
+      </c>
+      <c r="B4" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
+  FILTER(
+    {
+      MASTER!D2:D1000,
+      MASTER!A2:A1000
+    },
+    MASTER!F2:F1000 = 1,
+    MASTER!C2:C1000 = ""A"",
+    MATCH(
+      MASTER!A2:A1000,
+      FILTER(
+        IPPEXPN!A2:A1000,
+        IPPEXPN!C2:C1000 = 1,
+        REGEXMATCH(IPP"&amp;"EXPN!B2:B1000, ""Sex Offender"")
+      )
+    )
+  ),
+  ""SELECT Col1, COUNT(Col2)
+   GROUP BY Col1
+   ORDER BY COUNT(Col2) DESC
+   LIMIT 1
+   LABEL Col1 'Facility',
+         COUNT(Col2) 'Sex Offenders In Progress'"",
+  0
+)
+"),"Facility")</f>
+        <v>Facility</v>
+      </c>
+      <c r="B1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sex Offenders In Progress")</f>
+        <v>Sex Offenders In Progress</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
+        <v>Facility A</v>
+      </c>
+      <c r="B2" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
+  FILTER(
+    {
+      MASTER!D2:D1000,
+      MASTER!A2:A1000
+    },
+    MASTER!F2:F1000 = 1,
+    MASTER!C2:C1000 = ""A"",
+    MATCH(
+      MASTER!A2:A1000,
+      FILTER(
+        IPPEXPN!A2:A1000,
+        REGEXMATCH(IPPEXPN!B2:B1000,""Sex Offender"""&amp;")
+      )
+    )
+  ),
+  ""SELECT Col1, COUNT(Col2)
+   GROUP BY Col1
+   LABEL Col1 'Facility',
+         COUNT(Col2) 'Total Enrolled'""
+)
+"),"Facility")</f>
+        <v>Facility</v>
+      </c>
+      <c r="B1" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Total Enrolled")</f>
+        <v>Total Enrolled</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
+        <v>Facility A</v>
+      </c>
+      <c r="B2" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility B")</f>
+        <v>Facility B</v>
+      </c>
+      <c r="B3" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility D")</f>
+        <v>Facility D</v>
+      </c>
+      <c r="B4" s="5">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ST-0015: new inmate and program file updated with thought process
</commit_message>
<xml_diff>
--- a/InmateRosterDataFolder/Inmate Program Data.xlsx
+++ b/InmateRosterDataFolder/Inmate Program Data.xlsx
@@ -8,7 +8,8 @@
     <sheet state="visible" name="Question 1" sheetId="3" r:id="rId7"/>
     <sheet state="visible" name="Question 2" sheetId="4" r:id="rId8"/>
     <sheet state="visible" name="Question 3" sheetId="5" r:id="rId9"/>
-    <sheet state="visible" name="Question 5" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="Question 4" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="Question 5" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>MASDC#</t>
   </si>
@@ -121,6 +122,108 @@
   </si>
   <si>
     <t>Weapon Offenses</t>
+  </si>
+  <si>
+    <t>Question: We need a list of currently incarcerated Sex Offenders currently enrolled in the required Sex Offender training program.  
+Hint: Location part 1 (MASLC1) will = "A" when in a Correctional Facility. MASSOFF will = 1 if they're a Sex Offender. EXPPSTAT will = 'I' when in progress </t>
+  </si>
+  <si>
+    <t>Thought Process:
+Find the inmate name.
+Keep only Sex Offenders
+Keeps inmates currently housed in a correctional facility
+The fllter function will produces a list of Inmate IDs who:
+Are in progress (EXPPSTAT = 1)
+Are enrolled in a Sex Offender program.
+The match function will checks whether each inmate in MASTER appears in that filtered list.
+If found then returns a number.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result (Click on Cell A13 to show SQL query): </t>
+  </si>
+  <si>
+    <t>Question: We want to know the count of how many offenders in each facility have not received credit for completing the required training.   
+Hint: EXPNNCR will equal 1 if credit was awarded. </t>
+  </si>
+  <si>
+    <t>Thought Process:
+Creates a two-column virtual table using MASTER!D2:D,MASTER!A2:A
+Removes all non-Sex Offenders
+Keeps inmates currently housed in a correctional facility
+Produce a list of Inmate IDs who:
+Are currently in progress (EXPPSTAT = 1)
+Are enrolled in a Sex Offender program
+Have NOT received credit (EXPNNCR ≠ 1)
+Checks each inmate in MASTER
+Keeps only inmates who appear in the program list
+Groups offenders by Facility
+Counts how many offenders are in each group
+Create new label and display new header with data</t>
+  </si>
+  <si>
+    <t>Needed Clarification Questions:
+Is MASSOFF = 1 the only indicator used to classify an inmate as a Sex Offender, or are there additional flags or categories that should be considered?</t>
+  </si>
+  <si>
+    <t>Result:
+Only thought process, not able to produce query.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question: List of facilities with the highest number of Sex Offenders currently in progress. 
+Hint: To find the facilities with the highest number of Sex Offenders currently in progress, you may want to use a combination of SQL clauses to group the data appropriately and identify the facility with the most inmates in the 'in progress' status. </t>
+  </si>
+  <si>
+    <t>Thought Process: 
+Creates a two-column virtual table using MASTER!D2:D,MASTER!A2:A
+Removes all non-Sex Offenders
+Keeps inmates currently housed in a correctional facility
+Produce a list of Inmate IDs who:
+Are currently in progress (EXPPSTAT = 1)
+Are enrolled in a Sex Offender program</t>
+  </si>
+  <si>
+    <t>Needed Clarification Questions:
+How do we remove all non-Sex Offencers?
+How to produce a list of inmate with their ID?</t>
+  </si>
+  <si>
+    <t>Question: List all inmates who have completed at least one Sex Offender Program, along with their names and the total number of programs they've completed.
+Hint: To identify inmates who have completed at least one program, consider using an appropriate aggregate function and a HAVING clause.</t>
+  </si>
+  <si>
+    <t>Thought Process: 
+the question is asking summary by inmate.
+Go to IPPEXPN to find completions.
+Then connect those results to MASTER to get names</t>
+  </si>
+  <si>
+    <t>Needed Clarification Questions:
+How is completed program defined?
+Should repeated program completions be counted separately?</t>
+  </si>
+  <si>
+    <t>Result:
+Only thought process, not able to find result for this question</t>
+  </si>
+  <si>
+    <t>The percentage of offenders who have received credit for completing the required training by facility. 
+Hint: You'll need to use SQL to identify consecutive sequences of 'C' status for each Sex Offender and then find the longest streak.</t>
+  </si>
+  <si>
+    <t>Thought Process:
+The question asks for a percentage by facility, which means comparing two counts.
+Numerator: offenders who received credit for completing required training
+Denominator: offenders who were required / enrolled in that training
+Decide who counts:
+Only Sex Offenders
+Only offenders associated with a facility
+Only offenders who were part of the required training</t>
+  </si>
+  <si>
+    <t>Needed Clarification Questions:
+What defines the required training?
+How should offenders with multiple enrollments be treated?
+How should missing or inconsistent data be handled?</t>
   </si>
 </sst>
 </file>
@@ -268,6 +371,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -863,17 +970,36 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="str">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("FILTER(
-  MASTER!B2:B1005,
-  MASTER!F2:F1005 = 1,
-  MASTER!C2:C1005 = ""A"",
+  MASTER!B2:B1003,
+  MASTER!F2:F1003 = 1,
+  MASTER!C2:C1003 = ""A"",
     MATCH(
-      MASTER!A2:A1005,
+      MASTER!A2:A1003,
       FILTER(
-        IPPEXPN!A2:A1005,
-        IPPEXPN!C2:C1005 = 1,
-        REGEXMATCH(IPPEXPN!B2:B1005, ""Sex Offender"")
+        IPPEXPN!A2:A1003,
+        IPPEXPN!C2:C1003 = 1,
+        REGEXMATCH(IPPEXPN!B2:B1003, ""Sex Offender"")
       )
   )
 )
@@ -881,20 +1007,17 @@
         <v>Robert Lee</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="5" t="str">
+    <row r="9">
+      <c r="A9" s="5" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Daniel Anderson")</f>
         <v>Daniel Anderson</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
+    <row r="10">
+      <c r="A10" s="5" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Alex Han")</f>
         <v>Alex Han</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -912,65 +1035,26 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
-  FILTER(
-    {
-      MASTER!D2:D1000,
-      MASTER!A2:A1000
-    },
-    MASTER!F2:F1000 = 1,
-    MASTER!C2:C1000 = ""A"",
-    MATCH(
-      MASTER!A2:A1000,
-      FILTER(
-        IPPEXPN!A2:A1000,
-        IPPEXPN!C2:C1000 = 1,
-        IPPEXPN!D2:D10"&amp;"00 &lt;&gt; 1,
-        REGEXMATCH(IPPEXPN!B2:B1000, ""Sex Offender"")
-      )
-    )
-  ),
-  ""SELECT Col1, COUNT(Col2)
-   GROUP BY Col1
-   LABEL Col1 'Facility',
-         COUNT(Col2) 'Offenders Without Credit'""
-)"),"Facility")</f>
-        <v>Facility</v>
-      </c>
-      <c r="B1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Offenders Without Credit")</f>
-        <v>Offenders Without Credit</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
-        <v>Facility A</v>
-      </c>
-      <c r="B2" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility B")</f>
-        <v>Facility B</v>
-      </c>
-      <c r="B3" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
+      <c r="A3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility D")</f>
-        <v>Facility D</v>
-      </c>
-      <c r="B4" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -989,48 +1073,35 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
-  FILTER(
-    {
-      MASTER!D2:D1000,
-      MASTER!A2:A1000
-    },
-    MASTER!F2:F1000 = 1,
-    MASTER!C2:C1000 = ""A"",
-    MATCH(
-      MASTER!A2:A1000,
-      FILTER(
-        IPPEXPN!A2:A1000,
-        IPPEXPN!C2:C1000 = 1,
-        REGEXMATCH(IPP"&amp;"EXPN!B2:B1000, ""Sex Offender"")
-      )
-    )
-  ),
-  ""SELECT Col1, COUNT(Col2)
-   GROUP BY Col1
-   ORDER BY COUNT(Col2) DESC
-   LIMIT 1
-   LABEL Col1 'Facility',
-         COUNT(Col2) 'Sex Offenders In Progress'"",
-  0
-)
-"),"Facility")</f>
-        <v>Facility</v>
-      </c>
-      <c r="B1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sex Offenders In Progress")</f>
-        <v>Sex Offenders In Progress</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
-        <v>Facility A</v>
-      </c>
-      <c r="B2" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1049,64 +1120,58 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("QUERY(
-  FILTER(
-    {
-      MASTER!D2:D1000,
-      MASTER!A2:A1000
-    },
-    MASTER!F2:F1000 = 1,
-    MASTER!C2:C1000 = ""A"",
-    MATCH(
-      MASTER!A2:A1000,
-      FILTER(
-        IPPEXPN!A2:A1000,
-        REGEXMATCH(IPPEXPN!B2:B1000,""Sex Offender"""&amp;")
-      )
-    )
-  ),
-  ""SELECT Col1, COUNT(Col2)
-   GROUP BY Col1
-   LABEL Col1 'Facility',
-         COUNT(Col2) 'Total Enrolled'""
-)
-"),"Facility")</f>
-        <v>Facility</v>
-      </c>
-      <c r="B1" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Total Enrolled")</f>
-        <v>Total Enrolled</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility A")</f>
-        <v>Facility A</v>
-      </c>
-      <c r="B2" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility B")</f>
-        <v>Facility B</v>
-      </c>
-      <c r="B3" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Facility D")</f>
-        <v>Facility D</v>
-      </c>
-      <c r="B4" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>